<commit_message>
Updated the code examples - Openpyxl module - Days70-72
</commit_message>
<xml_diff>
--- a/days70-72/Financial Sample.xlsx
+++ b/days70-72/Financial Sample.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="1" windowHeight="7770" windowWidth="23595" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="7770" windowWidth="23595" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Finances 2017" sheetId="1" state="visible" r:id="rId1"/>
@@ -745,7 +745,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P703"/>
+  <dimension ref="A1:P705"/>
   <sheetViews>
     <sheetView topLeftCell="A681" workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
       <selection activeCell="O703" sqref="O703"/>
@@ -35821,6 +35821,7 @@
         <v>21</v>
       </c>
     </row>
+    <row r="702" spans="1:16"/>
     <row r="703" spans="1:16">
       <c r="L703">
         <f>SUM(L2:L702)</f>
@@ -35828,6 +35829,12 @@
       </c>
       <c r="M703">
         <f>SUM(L2:L704)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="705" spans="1:16">
+      <c r="L705">
+        <f>SUM(L2:L702)</f>
         <v/>
       </c>
     </row>

</xml_diff>